<commit_message>
Fetch CTA from SBTi & use LEI to check for validated targets (#292)
* First commit

* Update interfaces.py

* With test module

* Adjustments to example file and legend

* Added dummy value to LEI for transitional purposes

* Changed dummy value for LEI

* Added LEI to standard example portfolio

* Bumped version to 1.0.6 in pyproject.toml

* wording in docs and a test module

* Adding aggregation notebook for ready made scores

* Update to docs

* Docs fix

* More updates
</commit_message>
<xml_diff>
--- a/docs/PortfolioTemplate.xlsx
+++ b/docs/PortfolioTemplate.xlsx
@@ -1,21 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="23308"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="26026"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\daanm\Documents\temp\SBTi\documentation\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl$\Ubuntu-20.04\home\mountainrambler\SBTi\SBTi-finance-tool\docs\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="8" documentId="11_F842464B1A184FBFEBE833DDB0F5962AF954E04A" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{49F42B5B-49C9-46B1-A8EC-411BF06A182B}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{597F54FC-AAD6-4488-8D61-5FA72822E791}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="51600" windowHeight="17835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1776" yWindow="1896" windowWidth="16356" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="User input" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="191028" calcCompleted="0"/>
+  <calcPr calcId="191028"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -33,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="14">
   <si>
     <t>company_name</t>
   </si>
@@ -66,6 +66,15 @@
   </si>
   <si>
     <t>UK0000002</t>
+  </si>
+  <si>
+    <t>company_lei</t>
+  </si>
+  <si>
+    <t>JP0000000001</t>
+  </si>
+  <si>
+    <t>UK0000000002</t>
   </si>
 </sst>
 </file>
@@ -75,7 +84,7 @@
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
-  <fonts count="2">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -168,12 +177,13 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table7" displayName="Table7" ref="A1:G52" totalsRowShown="0">
-  <autoFilter ref="A1:G52" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{00000000-000C-0000-FFFF-FFFF00000000}" name="Table7" displayName="Table7" ref="A1:H52" totalsRowShown="0">
+  <autoFilter ref="A1:H52" xr:uid="{00000000-0009-0000-0100-000001000000}"/>
+  <tableColumns count="8">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0000-000001000000}" name="company_name"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0000-000002000000}" name="company_id"/>
     <tableColumn id="7" xr3:uid="{00000000-0010-0000-0000-000007000000}" name="company_isin"/>
+    <tableColumn id="8" xr3:uid="{E7FE8F50-51F5-4DF2-A5F4-F3E6163C7D17}" name="company_lei"/>
     <tableColumn id="4" xr3:uid="{00000000-0010-0000-0000-000004000000}" name="investment_value" dataCellStyle="Comma"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0000-000003000000}" name="engagement_targets"/>
     <tableColumn id="5" xr3:uid="{00000000-0010-0000-0000-000005000000}" name="additional_field_1"/>
@@ -446,23 +456,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:G52"/>
+  <dimension ref="A1:H52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.42578125" customWidth="1"/>
-    <col min="2" max="2" width="14.42578125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="17.44140625" customWidth="1"/>
+    <col min="2" max="2" width="14.44140625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="14" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="14.7109375" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="21.85546875" bestFit="1" customWidth="1"/>
-    <col min="6" max="7" width="19.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="14" customWidth="1"/>
+    <col min="5" max="5" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="21.88671875" bestFit="1" customWidth="1"/>
+    <col min="7" max="8" width="19.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -473,19 +484,22 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="2" spans="1:7">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A2" s="2" t="s">
         <v>7</v>
       </c>
@@ -495,11 +509,14 @@
       <c r="C2" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1">
+      <c r="D2" t="s">
+        <v>12</v>
+      </c>
+      <c r="E2" s="1">
         <v>1000000</v>
       </c>
     </row>
-    <row r="3" spans="1:7">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A3" s="4" t="s">
         <v>9</v>
       </c>
@@ -509,156 +526,159 @@
       <c r="C3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="1">
+      <c r="D3" t="s">
+        <v>13</v>
+      </c>
+      <c r="E3" s="1">
         <v>2500000</v>
       </c>
     </row>
-    <row r="4" spans="1:7">
-      <c r="D4" s="1"/>
-    </row>
-    <row r="5" spans="1:7">
-      <c r="D5" s="1"/>
-    </row>
-    <row r="6" spans="1:7">
-      <c r="D6" s="1"/>
-    </row>
-    <row r="7" spans="1:7">
-      <c r="D7" s="1"/>
-    </row>
-    <row r="8" spans="1:7">
-      <c r="D8" s="1"/>
-    </row>
-    <row r="9" spans="1:7">
-      <c r="D9" s="1"/>
-    </row>
-    <row r="10" spans="1:7">
-      <c r="D10" s="1"/>
-    </row>
-    <row r="11" spans="1:7">
-      <c r="D11" s="1"/>
-    </row>
-    <row r="12" spans="1:7">
-      <c r="D12" s="1"/>
-    </row>
-    <row r="13" spans="1:7">
-      <c r="D13" s="1"/>
-    </row>
-    <row r="14" spans="1:7">
-      <c r="D14" s="1"/>
-    </row>
-    <row r="15" spans="1:7">
-      <c r="D15" s="1"/>
-    </row>
-    <row r="16" spans="1:7">
-      <c r="D16" s="1"/>
-    </row>
-    <row r="17" spans="4:4">
-      <c r="D17" s="1"/>
-    </row>
-    <row r="18" spans="4:4">
-      <c r="D18" s="1"/>
-    </row>
-    <row r="19" spans="4:4">
-      <c r="D19" s="1"/>
-    </row>
-    <row r="20" spans="4:4">
-      <c r="D20" s="1"/>
-    </row>
-    <row r="21" spans="4:4">
-      <c r="D21" s="1"/>
-    </row>
-    <row r="22" spans="4:4">
-      <c r="D22" s="1"/>
-    </row>
-    <row r="23" spans="4:4">
-      <c r="D23" s="1"/>
-    </row>
-    <row r="24" spans="4:4">
-      <c r="D24" s="1"/>
-    </row>
-    <row r="25" spans="4:4">
-      <c r="D25" s="1"/>
-    </row>
-    <row r="26" spans="4:4">
-      <c r="D26" s="1"/>
-    </row>
-    <row r="27" spans="4:4">
-      <c r="D27" s="1"/>
-    </row>
-    <row r="28" spans="4:4">
-      <c r="D28" s="1"/>
-    </row>
-    <row r="29" spans="4:4">
-      <c r="D29" s="1"/>
-    </row>
-    <row r="30" spans="4:4">
-      <c r="D30" s="1"/>
-    </row>
-    <row r="31" spans="4:4">
-      <c r="D31" s="1"/>
-    </row>
-    <row r="32" spans="4:4">
-      <c r="D32" s="1"/>
-    </row>
-    <row r="33" spans="4:4">
-      <c r="D33" s="1"/>
-    </row>
-    <row r="34" spans="4:4">
-      <c r="D34" s="1"/>
-    </row>
-    <row r="35" spans="4:4">
-      <c r="D35" s="1"/>
-    </row>
-    <row r="36" spans="4:4">
-      <c r="D36" s="1"/>
-    </row>
-    <row r="37" spans="4:4">
-      <c r="D37" s="1"/>
-    </row>
-    <row r="38" spans="4:4">
-      <c r="D38" s="1"/>
-    </row>
-    <row r="39" spans="4:4">
-      <c r="D39" s="1"/>
-    </row>
-    <row r="40" spans="4:4">
-      <c r="D40" s="1"/>
-    </row>
-    <row r="41" spans="4:4">
-      <c r="D41" s="1"/>
-    </row>
-    <row r="42" spans="4:4">
-      <c r="D42" s="1"/>
-    </row>
-    <row r="43" spans="4:4">
-      <c r="D43" s="1"/>
-    </row>
-    <row r="44" spans="4:4">
-      <c r="D44" s="1"/>
-    </row>
-    <row r="45" spans="4:4">
-      <c r="D45" s="1"/>
-    </row>
-    <row r="46" spans="4:4">
-      <c r="D46" s="1"/>
-    </row>
-    <row r="47" spans="4:4">
-      <c r="D47" s="1"/>
-    </row>
-    <row r="48" spans="4:4">
-      <c r="D48" s="1"/>
-    </row>
-    <row r="49" spans="4:4">
-      <c r="D49" s="1"/>
-    </row>
-    <row r="50" spans="4:4">
-      <c r="D50" s="1"/>
-    </row>
-    <row r="51" spans="4:4">
-      <c r="D51" s="1"/>
-    </row>
-    <row r="52" spans="4:4">
-      <c r="D52" s="1"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E4" s="1"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E5" s="1"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E6" s="1"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E7" s="1"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E8" s="1"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E9" s="1"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E10" s="1"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E11" s="1"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E12" s="1"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E13" s="1"/>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E14" s="1"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E15" s="1"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="E16" s="1"/>
+    </row>
+    <row r="17" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E17" s="1"/>
+    </row>
+    <row r="18" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E18" s="1"/>
+    </row>
+    <row r="19" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E19" s="1"/>
+    </row>
+    <row r="20" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E20" s="1"/>
+    </row>
+    <row r="21" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E21" s="1"/>
+    </row>
+    <row r="22" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E22" s="1"/>
+    </row>
+    <row r="23" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E23" s="1"/>
+    </row>
+    <row r="24" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E24" s="1"/>
+    </row>
+    <row r="25" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E25" s="1"/>
+    </row>
+    <row r="26" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E26" s="1"/>
+    </row>
+    <row r="27" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E27" s="1"/>
+    </row>
+    <row r="28" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E28" s="1"/>
+    </row>
+    <row r="29" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E29" s="1"/>
+    </row>
+    <row r="30" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E30" s="1"/>
+    </row>
+    <row r="31" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E31" s="1"/>
+    </row>
+    <row r="32" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E32" s="1"/>
+    </row>
+    <row r="33" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E33" s="1"/>
+    </row>
+    <row r="34" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E34" s="1"/>
+    </row>
+    <row r="35" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E35" s="1"/>
+    </row>
+    <row r="36" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E36" s="1"/>
+    </row>
+    <row r="37" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E37" s="1"/>
+    </row>
+    <row r="38" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E38" s="1"/>
+    </row>
+    <row r="39" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E39" s="1"/>
+    </row>
+    <row r="40" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E40" s="1"/>
+    </row>
+    <row r="41" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E41" s="1"/>
+    </row>
+    <row r="42" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E42" s="1"/>
+    </row>
+    <row r="43" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E43" s="1"/>
+    </row>
+    <row r="44" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E44" s="1"/>
+    </row>
+    <row r="45" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E45" s="1"/>
+    </row>
+    <row r="46" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E46" s="1"/>
+    </row>
+    <row r="47" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E47" s="1"/>
+    </row>
+    <row r="48" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E48" s="1"/>
+    </row>
+    <row r="49" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E49" s="1"/>
+    </row>
+    <row r="50" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E50" s="1"/>
+    </row>
+    <row r="51" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E51" s="1"/>
+    </row>
+    <row r="52" spans="5:5" x14ac:dyDescent="0.3">
+      <c r="E52" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -669,21 +689,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="dokument" ma:contentTypeID="0x010100DEE3DD05F1781645A88261586288E143" ma:contentTypeVersion="8" ma:contentTypeDescription="Skapa ett nytt dokument." ma:contentTypeScope="" ma:versionID="10141bd3b7df6929ac2aab0d38ace983">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="84fd47fe-9509-4b60-beed-e31c94bc7d6c" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="679635ba64e6b0b974d32fba01d99d42" ns2:_="">
     <xsd:import namespace="84fd47fe-9509-4b60-beed-e31c94bc7d6c"/>
@@ -855,14 +860,52 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D062502D-5447-429F-99FE-9C021707C696}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FF9232B-D5F8-41D0-9ED5-473CE21EE010}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="84fd47fe-9509-4b60-beed-e31c94bc7d6c"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C607CFBC-7358-4C6E-8F9C-34365C4874E6}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{C607CFBC-7358-4C6E-8F9C-34365C4874E6}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9FF9232B-D5F8-41D0-9ED5-473CE21EE010}"/>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{D062502D-5447-429F-99FE-9C021707C696}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>